<commit_message>
improve scan list example
</commit_message>
<xml_diff>
--- a/common/ScanList_example.xlsx
+++ b/common/ScanList_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t xml:space="preserve">study_name</t>
   </si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">analyse</t>
   </si>
   <si>
+    <t xml:space="preserve">phaseDir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM</t>
+  </si>
+  <si>
     <t xml:space="preserve">sub-01</t>
   </si>
   <si>
@@ -81,6 +87,12 @@
   <si>
     <t xml:space="preserve">PGSE</t>
   </si>
+  <si>
+    <t xml:space="preserve">sub-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20251204_103047_20251111_CTD_P10_PL_20251204_Rat_CTD_1780_1_15</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,6 +135,7 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -134,13 +147,31 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -184,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,11 +224,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,6 +249,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -218,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -230,7 +329,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.38"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -267,11 +366,15 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -287,31 +390,31 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>1788</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -334,31 +437,31 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>1788</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -381,31 +484,31 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>1788</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -426,22 +529,40 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>1780</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
@@ -455,22 +576,40 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1780</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -29281,39 +29420,11 @@
       <c r="Z999" s="3"/>
       <c r="AA999" s="3"/>
     </row>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="3"/>
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
-      <c r="H1000" s="3"/>
-      <c r="I1000" s="3"/>
-      <c r="J1000" s="3"/>
-      <c r="K1000" s="3"/>
-      <c r="L1000" s="3"/>
-      <c r="M1000" s="3"/>
-      <c r="N1000" s="3"/>
-      <c r="O1000" s="3"/>
-      <c r="P1000" s="3"/>
-      <c r="Q1000" s="3"/>
-      <c r="R1000" s="3"/>
-      <c r="S1000" s="3"/>
-      <c r="T1000" s="3"/>
-      <c r="U1000" s="3"/>
-      <c r="V1000" s="3"/>
-      <c r="W1000" s="3"/>
-      <c r="X1000" s="3"/>
-      <c r="Y1000" s="3"/>
-      <c r="Z1000" s="3"/>
-      <c r="AA1000" s="3"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G4" type="list">
-      <formula1>"PGSE,T2W,T1W,STE"</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G6" type="list">
+      <formula1>"PGSE,T2W,T1W,STE,SPECIAL"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>